<commit_message>
in the middle of tutorial part3
</commit_message>
<xml_diff>
--- a/Django.xlsx
+++ b/Django.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Personal\Learn\Web-development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB3AB45-16B0-4DC0-952F-1BE959D9F9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CBE4E5-D10B-441B-AFB0-3413D3BE1F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -556,7 +556,11 @@
         <v>52</v>
       </c>
       <c r="C3" s="6">
-        <f>A32</f>
+        <f>$A32</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3" s="6">
+        <f>$A32</f>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -567,6 +571,9 @@
       <c r="C4" s="5">
         <v>0.49374999999999997</v>
       </c>
+      <c r="D4" s="5">
+        <v>0.54652777777777783</v>
+      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
@@ -575,6 +582,9 @@
       <c r="C5" s="5">
         <v>0.56180555555555556</v>
       </c>
+      <c r="D5" s="5">
+        <v>0.60902777777777783</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -583,16 +593,25 @@
       <c r="C6" s="5">
         <v>0.7284722222222223</v>
       </c>
+      <c r="D6" s="5">
+        <v>0.65138888888888891</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="D7" s="5">
+        <v>0.66805555555555562</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="D8" s="5">
+        <v>0.84375</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -629,40 +648,43 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="5">
         <v>0.8618055555555556</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="5">
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -670,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1.2</v>
       </c>
@@ -678,12 +700,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f>A27+1</f>
         <v>2.1</v>
@@ -692,7 +714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f>A28+1</f>
         <v>2.2000000000000002</v>

</xml_diff>

<commit_message>
wrapped the project in venv; replace the  app with its python package version
</commit_message>
<xml_diff>
--- a/Django.xlsx
+++ b/Django.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Personal\Learn\Web-development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D31788-474C-4740-B909-86D0B58ED4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B63FAA-243B-4D11-B43D-E71D78C66C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -542,7 +542,7 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C1" s="4">
         <v>45261</v>
       </c>
@@ -562,8 +562,12 @@
         <f>F1+1</f>
         <v>45265</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="4">
+        <f>G1+1</f>
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>52</v>
       </c>
@@ -587,8 +591,12 @@
         <f>$A32</f>
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="6">
+        <f>$A32</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>46</v>
       </c>
@@ -607,8 +615,11 @@
       <c r="G4" s="5">
         <v>0.4381944444444445</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>47</v>
       </c>
@@ -627,8 +638,11 @@
       <c r="G5" s="5">
         <v>0.60138888888888886</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
@@ -647,8 +661,11 @@
       <c r="G6" s="5">
         <v>0.65763888888888888</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
@@ -662,8 +679,11 @@
       <c r="G7" s="5">
         <v>0.68055555555555547</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
@@ -677,8 +697,11 @@
       <c r="G8" s="5">
         <v>0.70624999999999993</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>47</v>
       </c>
@@ -688,8 +711,11 @@
       <c r="G9" s="5">
         <v>0.74791666666666667</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="5">
+        <v>0.64930555555555558</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>48</v>
       </c>
@@ -699,53 +725,56 @@
       <c r="G10" s="5">
         <v>0.81944444444444453</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="5">
+        <v>0.79999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
@@ -764,13 +793,16 @@
       <c r="G21" s="5">
         <v>0.87013888888888891</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="5">
+        <v>0.83124999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -778,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1.2</v>
       </c>
@@ -786,12 +818,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f>A27+1</f>
         <v>2.1</v>
@@ -800,7 +832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f>A28+1</f>
         <v>2.2000000000000002</v>

</xml_diff>